<commit_message>
Coh is included in all plots, and I have fixed some other minor things
</commit_message>
<xml_diff>
--- a/Which_nuclei_seen_in_spectra.xlsx
+++ b/Which_nuclei_seen_in_spectra.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/d50fdffd1f97c7a6/Dokumenter/Master/Master-project-code/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="183" documentId="8_{396205E7-18F3-7246-A276-F5082CCA7CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{CA859DE4-3FCC-784C-960E-95E247EA3EA0}"/>
+  <xr:revisionPtr revIDLastSave="406" documentId="8_{396205E7-18F3-7246-A276-F5082CCA7CA5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{13DF4CD2-D5FF-434B-BF39-0EA59DBEF291}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{45685930-CF24-F34F-B451-8FBF1C99710B}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="59">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="350" uniqueCount="81">
   <si>
     <t>Ni01</t>
   </si>
@@ -213,6 +213,72 @@
   </si>
   <si>
     <t>87Y</t>
+  </si>
+  <si>
+    <t>87mY</t>
+  </si>
+  <si>
+    <t>88Y</t>
+  </si>
+  <si>
+    <t>88Nb</t>
+  </si>
+  <si>
+    <t>88Zr</t>
+  </si>
+  <si>
+    <t>89Nb</t>
+  </si>
+  <si>
+    <t>89Zr</t>
+  </si>
+  <si>
+    <t>90mY</t>
+  </si>
+  <si>
+    <t>90Nb</t>
+  </si>
+  <si>
+    <t>91mNb</t>
+  </si>
+  <si>
+    <t>92mNb</t>
+  </si>
+  <si>
+    <t>95mNb</t>
+  </si>
+  <si>
+    <t>95Nb</t>
+  </si>
+  <si>
+    <t>95Zr</t>
+  </si>
+  <si>
+    <t>96Nb</t>
+  </si>
+  <si>
+    <t>Not able to fit</t>
+  </si>
+  <si>
+    <t xml:space="preserve">n </t>
+  </si>
+  <si>
+    <t>n***</t>
+  </si>
+  <si>
+    <t>***Not able to run the peak fit file</t>
+  </si>
+  <si>
+    <t>yy, wrong</t>
+  </si>
+  <si>
+    <t>yy, have removed it fros xs</t>
+  </si>
+  <si>
+    <t>yy, have removed it from xs</t>
+  </si>
+  <si>
+    <t>Isomeren og gs deler topp. Ser antaglig ikke gs...</t>
   </si>
 </sst>
 </file>
@@ -633,10 +699,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{F6BD05D9-F62B-A146-87F6-97D4C7B61A5A}">
-  <dimension ref="A3:K364"/>
+  <dimension ref="A3:L363"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A11" workbookViewId="0">
-      <selection activeCell="F32" sqref="F32"/>
+    <sheetView tabSelected="1" topLeftCell="A33" zoomScale="137" zoomScaleNormal="150" workbookViewId="0">
+      <selection activeCell="E48" sqref="E48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -669,6 +735,11 @@
         <v>45</v>
       </c>
     </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" t="s">
+        <v>76</v>
+      </c>
+    </row>
     <row r="12" spans="1:6" x14ac:dyDescent="0.2">
       <c r="B12" s="1" t="s">
         <v>0</v>
@@ -696,8 +767,8 @@
       <c r="C13" t="s">
         <v>38</v>
       </c>
-      <c r="D13" s="2" t="s">
-        <v>39</v>
+      <c r="D13" s="5" t="s">
+        <v>40</v>
       </c>
       <c r="E13" t="s">
         <v>40</v>
@@ -766,7 +837,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="17" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A17" s="1" t="s">
         <v>41</v>
       </c>
@@ -786,7 +857,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="18" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A18" s="1" t="s">
         <v>9</v>
       </c>
@@ -806,7 +877,7 @@
         <v>42</v>
       </c>
     </row>
-    <row r="19" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A19" s="1" t="s">
         <v>10</v>
       </c>
@@ -826,15 +897,15 @@
         <v>42</v>
       </c>
     </row>
-    <row r="20" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A20" s="1" t="s">
         <v>11</v>
       </c>
       <c r="B20" t="s">
         <v>38</v>
       </c>
-      <c r="C20" s="3" t="s">
-        <v>39</v>
+      <c r="C20" s="4" t="s">
+        <v>40</v>
       </c>
       <c r="D20" t="s">
         <v>38</v>
@@ -846,7 +917,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="21" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A21" s="1" t="s">
         <v>12</v>
       </c>
@@ -866,7 +937,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="22" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A22" s="1" t="s">
         <v>13</v>
       </c>
@@ -886,7 +957,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="23" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A23" s="1" t="s">
         <v>14</v>
       </c>
@@ -906,16 +977,16 @@
         <v>40</v>
       </c>
     </row>
-    <row r="24" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A24" s="1"/>
       <c r="B24" s="4"/>
       <c r="F24" s="6"/>
     </row>
-    <row r="25" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A25" s="1"/>
       <c r="F25" s="6"/>
     </row>
-    <row r="26" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A26" s="1"/>
       <c r="B26" s="1" t="s">
         <v>19</v>
@@ -948,7 +1019,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="27" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A27" s="1" t="s">
         <v>28</v>
       </c>
@@ -982,8 +1053,11 @@
       <c r="K27" s="5" t="s">
         <v>40</v>
       </c>
-    </row>
-    <row r="28" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="L27" s="2" t="s">
+        <v>80</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A28" s="1" t="s">
         <v>29</v>
       </c>
@@ -1018,7 +1092,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="29" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A29" s="1" t="s">
         <v>30</v>
       </c>
@@ -1053,21 +1127,21 @@
         <v>38</v>
       </c>
     </row>
-    <row r="30" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A30" s="1" t="s">
         <v>31</v>
       </c>
-      <c r="B30" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="C30" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="D30" s="2" t="s">
-        <v>39</v>
-      </c>
-      <c r="E30" s="2" t="s">
-        <v>39</v>
+      <c r="B30" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="C30" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="D30" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="E30" s="6" t="s">
+        <v>40</v>
       </c>
       <c r="F30" s="6" t="s">
         <v>40</v>
@@ -1084,11 +1158,11 @@
       <c r="J30" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="K30" s="7" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="31" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="K30" s="6" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A31" s="1" t="s">
         <v>32</v>
       </c>
@@ -1123,7 +1197,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="32" spans="1:11" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A32" s="1"/>
       <c r="F32" s="6"/>
     </row>
@@ -1312,67 +1386,534 @@
       <c r="A44" s="1" t="s">
         <v>57</v>
       </c>
+      <c r="B44" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="C44" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D44" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E44" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F44" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G44" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H44" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I44" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J44" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K44" s="4" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="45" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A45" s="1" t="s">
         <v>58</v>
       </c>
+      <c r="B45" s="5"/>
+      <c r="C45" s="5"/>
+      <c r="D45" s="5"/>
+      <c r="E45" s="5"/>
+      <c r="F45" s="5"/>
+      <c r="G45" s="5"/>
+      <c r="H45" s="5"/>
+      <c r="I45" s="5"/>
+      <c r="J45" s="5"/>
+      <c r="K45" s="5"/>
     </row>
     <row r="46" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A46" s="1"/>
+      <c r="A46" s="1" t="s">
+        <v>59</v>
+      </c>
+      <c r="C46" s="5"/>
+      <c r="D46" s="5"/>
+      <c r="E46" s="5"/>
+      <c r="F46" s="5"/>
+      <c r="G46" s="5"/>
+      <c r="H46" s="5"/>
+      <c r="I46" s="5"/>
+      <c r="J46" s="5"/>
+      <c r="K46" s="5"/>
     </row>
     <row r="47" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A47" s="1"/>
+      <c r="A47" s="1" t="s">
+        <v>61</v>
+      </c>
+      <c r="B47" t="s">
+        <v>74</v>
+      </c>
+      <c r="C47" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D47" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E47" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F47" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G47" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H47" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I47" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="J47" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="K47" s="5" t="s">
+        <v>40</v>
+      </c>
     </row>
     <row r="48" spans="1:11" x14ac:dyDescent="0.2">
-      <c r="A48" s="1"/>
-    </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A49" s="1"/>
-    </row>
-    <row r="50" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A50" s="1"/>
-    </row>
-    <row r="51" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A51" s="1"/>
-    </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A52" s="1"/>
-    </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A53" s="1"/>
-    </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A54" s="1"/>
-    </row>
-    <row r="55" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A55" s="1"/>
-    </row>
-    <row r="56" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A56" s="1"/>
-    </row>
-    <row r="57" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A57" s="1"/>
-    </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A58" s="1"/>
-    </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A59" s="1"/>
-    </row>
-    <row r="60" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A48" s="1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B48" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="C48" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="D48" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="E48" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="F48" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="G48" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H48" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I48" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J48" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K48" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="49" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A49" s="1" t="s">
+        <v>60</v>
+      </c>
+      <c r="B49" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C49" s="4" t="s">
+        <v>38</v>
+      </c>
+      <c r="D49" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="E49" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="F49" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G49" s="5" t="s">
+        <v>46</v>
+      </c>
+      <c r="H49" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I49" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J49" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K49" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="50" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A50" s="1" t="s">
+        <v>63</v>
+      </c>
+      <c r="B50" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C50" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="D50" s="5" t="s">
+        <v>74</v>
+      </c>
+      <c r="E50" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="F50" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G50" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H50" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I50" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J50" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K50" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="51" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A51" s="1" t="s">
+        <v>64</v>
+      </c>
+      <c r="B51" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C51" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D51" s="3" t="s">
+        <v>79</v>
+      </c>
+      <c r="E51" s="3" t="s">
+        <v>78</v>
+      </c>
+      <c r="F51" s="5" t="s">
+        <v>40</v>
+      </c>
+      <c r="G51" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="H51" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I51" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J51" s="2" t="s">
+        <v>77</v>
+      </c>
+      <c r="K51" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="52" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A52" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B52" t="s">
+        <v>38</v>
+      </c>
+      <c r="C52" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="D52" t="s">
+        <v>38</v>
+      </c>
+      <c r="E52" t="s">
+        <v>74</v>
+      </c>
+      <c r="F52" t="s">
+        <v>40</v>
+      </c>
+      <c r="G52" t="s">
+        <v>38</v>
+      </c>
+      <c r="H52" t="s">
+        <v>38</v>
+      </c>
+      <c r="I52" t="s">
+        <v>38</v>
+      </c>
+      <c r="J52" s="3" t="s">
+        <v>39</v>
+      </c>
+      <c r="K52" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="53" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A53" s="1" t="s">
+        <v>66</v>
+      </c>
+      <c r="B53" t="s">
+        <v>38</v>
+      </c>
+      <c r="C53" t="s">
+        <v>38</v>
+      </c>
+      <c r="D53" t="s">
+        <v>38</v>
+      </c>
+      <c r="E53" t="s">
+        <v>38</v>
+      </c>
+      <c r="F53" t="s">
+        <v>38</v>
+      </c>
+      <c r="G53" t="s">
+        <v>38</v>
+      </c>
+      <c r="H53" t="s">
+        <v>38</v>
+      </c>
+      <c r="I53" t="s">
+        <v>38</v>
+      </c>
+      <c r="J53" t="s">
+        <v>38</v>
+      </c>
+      <c r="K53" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="54" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A54" s="1" t="s">
+        <v>67</v>
+      </c>
+      <c r="B54" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="C54" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="D54" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="E54" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="F54" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="G54" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="H54" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="I54" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="J54" s="2" t="s">
+        <v>73</v>
+      </c>
+      <c r="K54" s="2" t="s">
+        <v>73</v>
+      </c>
+    </row>
+    <row r="55" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A55" s="1" t="s">
+        <v>68</v>
+      </c>
+      <c r="B55" t="s">
+        <v>38</v>
+      </c>
+      <c r="C55" t="s">
+        <v>38</v>
+      </c>
+      <c r="D55" t="s">
+        <v>38</v>
+      </c>
+      <c r="E55" t="s">
+        <v>38</v>
+      </c>
+      <c r="F55" t="s">
+        <v>38</v>
+      </c>
+      <c r="G55" t="s">
+        <v>38</v>
+      </c>
+      <c r="H55" t="s">
+        <v>38</v>
+      </c>
+      <c r="I55" t="s">
+        <v>38</v>
+      </c>
+      <c r="J55" t="s">
+        <v>38</v>
+      </c>
+      <c r="K55" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="56" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A56" s="1" t="s">
+        <v>69</v>
+      </c>
+      <c r="B56" t="s">
+        <v>38</v>
+      </c>
+      <c r="C56" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D56" t="s">
+        <v>38</v>
+      </c>
+      <c r="E56" t="s">
+        <v>38</v>
+      </c>
+      <c r="F56" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G56" t="s">
+        <v>38</v>
+      </c>
+      <c r="H56" t="s">
+        <v>38</v>
+      </c>
+      <c r="I56" t="s">
+        <v>38</v>
+      </c>
+      <c r="J56" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K56" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="57" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A57" s="1" t="s">
+        <v>70</v>
+      </c>
+      <c r="B57" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C57" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="D57" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="E57" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="F57" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G57" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="H57" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="I57" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="J57" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="K57" s="5" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="58" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A58" s="1" t="s">
+        <v>71</v>
+      </c>
+      <c r="B58" s="5" t="s">
+        <v>38</v>
+      </c>
+      <c r="C58" t="s">
+        <v>38</v>
+      </c>
+      <c r="D58" t="s">
+        <v>38</v>
+      </c>
+      <c r="E58" t="s">
+        <v>38</v>
+      </c>
+      <c r="F58" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="G58" t="s">
+        <v>38</v>
+      </c>
+      <c r="H58" t="s">
+        <v>38</v>
+      </c>
+      <c r="I58" t="s">
+        <v>38</v>
+      </c>
+      <c r="J58" t="s">
+        <v>38</v>
+      </c>
+      <c r="K58" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="59" spans="1:11" x14ac:dyDescent="0.2">
+      <c r="A59" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B59" t="s">
+        <v>38</v>
+      </c>
+      <c r="C59" t="s">
+        <v>38</v>
+      </c>
+      <c r="D59" t="s">
+        <v>38</v>
+      </c>
+      <c r="E59" t="s">
+        <v>38</v>
+      </c>
+      <c r="F59" t="s">
+        <v>40</v>
+      </c>
+      <c r="G59" t="s">
+        <v>38</v>
+      </c>
+      <c r="H59" t="s">
+        <v>38</v>
+      </c>
+      <c r="I59" t="s">
+        <v>38</v>
+      </c>
+      <c r="J59" t="s">
+        <v>38</v>
+      </c>
+      <c r="K59" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="60" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A60" s="1"/>
     </row>
-    <row r="61" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A61" s="1"/>
     </row>
-    <row r="62" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A62" s="1"/>
     </row>
-    <row r="63" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A63" s="1"/>
     </row>
-    <row r="64" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:11" x14ac:dyDescent="0.2">
       <c r="A64" s="1"/>
     </row>
     <row r="65" spans="1:1" x14ac:dyDescent="0.2">
@@ -2271,9 +2812,6 @@
     </row>
     <row r="363" spans="1:1" x14ac:dyDescent="0.2">
       <c r="A363" s="1"/>
-    </row>
-    <row r="364" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A364" s="1"/>
     </row>
   </sheetData>
   <phoneticPr fontId="2" type="noConversion"/>

</xml_diff>